<commit_message>
server: tableManager ReadPassList() 수정
pass_list 시트에 limit_exp_daily_mission, level_repeated_reward 컬럼 추가 됨에 따른 수정
</commit_message>
<xml_diff>
--- a/Server/Server/GameData/Pass.xlsx
+++ b/Server/Server/GameData/Pass.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Download2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92E73C3-215C-42C1-B8C9-47FE7107CFD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1918BD-557D-4738-9CA5-4CBE9B45CE73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27990" windowHeight="16440" tabRatio="535" activeTab="3" xr2:uid="{E3B10073-6739-413D-9047-29D24A9ED330}"/>
+    <workbookView xWindow="5535" yWindow="2700" windowWidth="15465" windowHeight="13110" tabRatio="535" firstSheet="1" activeTab="2" xr2:uid="{E3B10073-6739-413D-9047-29D24A9ED330}"/>
   </bookViews>
   <sheets>
     <sheet name="Pass_Info" sheetId="4" r:id="rId1"/>
@@ -39,6 +39,33 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={02285BED-D805-4C5D-B344-7A602816A460}</author>
+    <author>tc={983CDA3A-21D9-4FC0-A46E-71C8B9484707}</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{02285BED-D805-4C5D-B344-7A602816A460}">
+      <text>
+        <t>[스레드 댓글]
+사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
+댓글:
+    일일미션 획득 경험치 한도</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="1" shapeId="0" xr:uid="{983CDA3A-21D9-4FC0-A46E-71C8B9484707}">
+      <text>
+        <t>[스레드 댓글]
+사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
+댓글:
+    반복보상 시작되는 패스 레벨</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={A63D4460-39A8-44C3-8C3B-C0AB19CB2BC3}</author>
@@ -85,7 +112,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={06EDA498-2F71-4579-9D6B-A579ACC4823E}</author>
@@ -176,7 +203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="85">
   <si>
     <t>Index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -490,6 +517,14 @@
   </si>
   <si>
     <t>Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level_Repeated_Reward</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Limit_Exp_Daily_Mission</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1001,6 +1036,17 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C1" dT="2025-02-11T02:42:07.46" personId="{36C43E8F-E806-4672-A3DE-BA0E07A7B13D}" id="{02285BED-D805-4C5D-B344-7A602816A460}">
+    <text>일일미션 획득 경험치 한도</text>
+  </threadedComment>
+  <threadedComment ref="D1" dT="2025-02-11T02:42:34.35" personId="{36C43E8F-E806-4672-A3DE-BA0E07A7B13D}" id="{983CDA3A-21D9-4FC0-A46E-71C8B9484707}">
+    <text>반복보상 시작되는 패스 레벨</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="C1" dT="2024-11-14T14:17:45.66" personId="{36C43E8F-E806-4672-A3DE-BA0E07A7B13D}" id="{A63D4460-39A8-44C3-8C3B-C0AB19CB2BC3}">
     <text>10레벨 초과 시, 레벨 10 유지&amp; 보상 지급</text>
   </threadedComment>
@@ -1018,7 +1064,7 @@
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="A1" dT="2025-02-10T02:34:23.59" personId="{36C43E8F-E806-4672-A3DE-BA0E07A7B13D}" id="{06EDA498-2F71-4579-9D6B-A579ACC4823E}">
     <text xml:space="preserve">600000 = 미션 전용
@@ -1208,50 +1254,65 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC616978-B69C-4F7D-8301-6F88E773EBCB}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC616978-B69C-4F7D-8301-6F88E773EBCB}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>601</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
+        <v>100</v>
+      </c>
+      <c r="D2" s="3">
+        <v>21</v>
+      </c>
+      <c r="E2" s="4">
         <v>45573</v>
       </c>
-      <c r="D2" s="4">
+      <c r="F2" s="4">
         <v>72686</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1259,8 +1320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A74E4F3-3BB8-4CF3-AC0A-3F86C309575D}">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2274,7 +2335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4561621-BAF4-4FB5-8F15-B71B1A49C200}">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>

</xml_diff>